<commit_message>
finish table, create scheme, first seminar homework is done
</commit_message>
<xml_diff>
--- a/Семинар 1/ДЗ Список фильмов.xlsx
+++ b/Семинар 1/ДЗ Список фильмов.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист1 (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId3"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
   <si>
     <t>Фильмы</t>
   </si>
@@ -43,6 +44,84 @@
   </si>
   <si>
     <t>Имя Актера</t>
+  </si>
+  <si>
+    <t>Человек-Паук</t>
+  </si>
+  <si>
+    <t>Тоби Магуайр</t>
+  </si>
+  <si>
+    <t>Фантастика</t>
+  </si>
+  <si>
+    <t>Зеленая книга</t>
+  </si>
+  <si>
+    <t>Виго Мортенсен</t>
+  </si>
+  <si>
+    <t>Один дома</t>
+  </si>
+  <si>
+    <t>Комедия</t>
+  </si>
+  <si>
+    <t>Никто</t>
+  </si>
+  <si>
+    <t>Главный герой</t>
+  </si>
+  <si>
+    <t>Боевик</t>
+  </si>
+  <si>
+    <t>Драма</t>
+  </si>
+  <si>
+    <t>Райан Рейнольдс</t>
+  </si>
+  <si>
+    <t>Приключения</t>
+  </si>
+  <si>
+    <t>Маколей Калкин</t>
+  </si>
+  <si>
+    <t>Боб Оденкёрк</t>
+  </si>
+  <si>
+    <t>Темный рыцарь</t>
+  </si>
+  <si>
+    <t>Кристиан Бейл</t>
+  </si>
+  <si>
+    <t>Пираты Карибского моря</t>
+  </si>
+  <si>
+    <t>Джонни Депп</t>
+  </si>
+  <si>
+    <t>Фентези</t>
+  </si>
+  <si>
+    <t>Звездные войны</t>
+  </si>
+  <si>
+    <t>Индиана Джонс</t>
+  </si>
+  <si>
+    <t>Марк Хэммил</t>
+  </si>
+  <si>
+    <t>Харрисон Форд</t>
+  </si>
+  <si>
+    <t>Логан</t>
+  </si>
+  <si>
+    <t>Хью Джекман</t>
   </si>
 </sst>
 </file>
@@ -404,16 +483,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
+    <col min="14" max="14" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14">
@@ -460,112 +540,192 @@
       <c r="B5" s="2">
         <v>0</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2002</v>
+      </c>
       <c r="I5" s="2">
         <v>0</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="M5" s="2">
         <v>0</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:14">
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2018</v>
+      </c>
       <c r="I6" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="M6" s="2">
         <v>1</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="2:14">
       <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1990</v>
+      </c>
       <c r="I7" s="2">
         <v>2</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M7" s="2">
         <v>2</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="2:14">
       <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2021</v>
+      </c>
       <c r="I8" s="2">
         <v>3</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="M8" s="2">
         <v>3</v>
       </c>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="2:14">
       <c r="B9" s="2">
         <v>4</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2021</v>
+      </c>
       <c r="I9" s="2">
         <v>4</v>
       </c>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="M9" s="2">
         <v>4</v>
       </c>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="2:14">
       <c r="B10" s="2">
         <v>5</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2008</v>
+      </c>
       <c r="I10" s="2">
         <v>5</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="M10" s="2">
         <v>5</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="2">
         <v>6</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2003</v>
+      </c>
       <c r="I11" s="2">
         <v>6</v>
       </c>
@@ -573,16 +733,26 @@
       <c r="M11" s="2">
         <v>6</v>
       </c>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="2">
         <v>7</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1977</v>
+      </c>
       <c r="I12" s="2">
         <v>7</v>
       </c>
@@ -590,16 +760,26 @@
       <c r="M12" s="2">
         <v>7</v>
       </c>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="2:14">
       <c r="B13" s="2">
         <v>8</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1981</v>
+      </c>
       <c r="I13" s="2">
         <v>8</v>
       </c>
@@ -607,16 +787,26 @@
       <c r="M13" s="2">
         <v>8</v>
       </c>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="2:14">
       <c r="B14" s="2">
         <v>9</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2017</v>
+      </c>
       <c r="I14" s="2">
         <v>9</v>
       </c>
@@ -624,7 +814,9 @@
       <c r="M14" s="2">
         <v>9</v>
       </c>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="2:14">
       <c r="B15" s="3"/>
@@ -669,9 +861,400 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:N19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
+    <col min="14" max="14" width="30.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2002</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1990</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="2">
+        <v>3</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="2">
+        <v>4</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2008</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" s="2">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2003</v>
+      </c>
+      <c r="I11" s="2">
+        <v>6</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="M11" s="2">
+        <v>6</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" s="2">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1977</v>
+      </c>
+      <c r="I12" s="2">
+        <v>7</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="M12" s="2">
+        <v>7</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="2">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1981</v>
+      </c>
+      <c r="I13" s="2">
+        <v>8</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="M13" s="2">
+        <v>8</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="2">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2017</v>
+      </c>
+      <c r="I14" s="2">
+        <v>9</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="M14" s="2">
+        <v>9</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D14">
+      <formula1>$J$5:$J$14</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E14">
+      <formula1>$N$5:$N$14</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
@@ -680,7 +1263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>